<commit_message>
Updated Pyramid with correct Layer 1 height
</commit_message>
<xml_diff>
--- a/Case Studies/Pyramid/Print times.xlsx
+++ b/Case Studies/Pyramid/Print times.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\UT AUSTIN\Sha Lab\Research\Placement\Placement\Case Studies\Pyramid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhw542\Documents\Coding\Placement\Case Studies\Pyramid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A774C610-2BB6-4FE4-B920-E2BEC73E3220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE137FE-45AD-40F3-81EB-69A3705C0DA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F521B8F1-06A0-48AF-9281-F1564FF20E0F}"/>
   </bookViews>
@@ -20,16 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -106,7 +96,7 @@
     <t>Layer 3</t>
   </si>
   <si>
-    <t>Layer 4</t>
+    <t>Layer 0</t>
   </si>
 </sst>
 </file>
@@ -473,35 +463,35 @@
   <dimension ref="A1:W17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="G1" s="2" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="M1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="S1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
@@ -597,11 +587,11 @@
         <v>2</v>
       </c>
       <c r="J3">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="K3">
         <f>((H3*24)+I3)*60+J3</f>
-        <v>1623</v>
+        <v>1579</v>
       </c>
       <c r="M3" t="s">
         <v>20</v>
@@ -660,14 +650,14 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="J4">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K17" si="1">((H4*24)+I4)*60+J4</f>
-        <v>2235</v>
+        <f t="shared" ref="K4:K14" si="1">((H4*24)+I4)*60+J4</f>
+        <v>1937</v>
       </c>
       <c r="M4" t="s">
         <v>2</v>
@@ -698,7 +688,7 @@
         <v>21</v>
       </c>
       <c r="W4">
-        <f t="shared" ref="W4:W17" si="3">((T4*24)+U4)*60+V4</f>
+        <f t="shared" ref="W4" si="3">((T4*24)+U4)*60+V4</f>
         <v>141</v>
       </c>
     </row>
@@ -726,14 +716,14 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J5">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="K5">
         <f t="shared" si="1"/>
-        <v>375</v>
+        <v>158</v>
       </c>
       <c r="M5" t="s">
         <v>1</v>
@@ -773,17 +763,17 @@
         <v>3</v>
       </c>
       <c r="H6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="J6">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="K6">
         <f t="shared" si="1"/>
-        <v>2973</v>
+        <v>2528</v>
       </c>
       <c r="M6" t="s">
         <v>3</v>
@@ -823,17 +813,17 @@
         <v>4</v>
       </c>
       <c r="H7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K7">
         <f t="shared" si="1"/>
-        <v>4800</v>
+        <v>3306</v>
       </c>
       <c r="M7" t="s">
         <v>4</v>
@@ -876,14 +866,14 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J8">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="K8">
         <f>((H8*24)+I8)*60+J8</f>
-        <v>372</v>
+        <v>266</v>
       </c>
       <c r="M8" t="s">
         <v>5</v>
@@ -926,14 +916,14 @@
         <v>1</v>
       </c>
       <c r="I9">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J9">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K9">
         <f t="shared" si="1"/>
-        <v>2198</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
@@ -957,17 +947,17 @@
         <v>7</v>
       </c>
       <c r="H10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="J10">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="K10">
         <f t="shared" si="1"/>
-        <v>3638</v>
+        <v>2763</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
@@ -994,14 +984,14 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="J11">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="K11">
         <f>((H11*24)+I11)*60+J11</f>
-        <v>422</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
@@ -1028,14 +1018,14 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="J12">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="K12">
         <f t="shared" si="1"/>
-        <v>1331</v>
+        <v>528</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
@@ -1059,17 +1049,17 @@
         <v>10</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J13">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="K13">
         <f t="shared" si="1"/>
-        <v>2009</v>
+        <v>649</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -1096,14 +1086,14 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J14">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="K14">
         <f t="shared" si="1"/>
-        <v>286</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>